<commit_message>
Multi Reporting Time and Gate Close Time Functionality added,Each Candidate's Exam date function created based no of Days
</commit_message>
<xml_diff>
--- a/dataentry/uploaded_excel_files/cgle_2019_tier_1.xlsx
+++ b/dataentry/uploaded_excel_files/cgle_2019_tier_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>ac_main_title</t>
   </si>
@@ -42,12 +42,6 @@
     <t>post_preference</t>
   </si>
   <si>
-    <t>repotime</t>
-  </si>
-  <si>
-    <t>gateclose</t>
-  </si>
-  <si>
     <t>venue1_title</t>
   </si>
   <si>
@@ -195,12 +189,6 @@
     <t>01111999</t>
   </si>
   <si>
-    <t>7.30 AM</t>
-  </si>
-  <si>
-    <t>8.30 AM</t>
-  </si>
-  <si>
     <t>iON Digital Zone iDZ  Kundrathur</t>
   </si>
   <si>
@@ -240,64 +228,22 @@
     <t>Karimnagar</t>
   </si>
   <si>
-    <t>13061999</t>
-  </si>
-  <si>
-    <t>Warangal</t>
-  </si>
-  <si>
-    <t>02051996</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Coimbatore</t>
-  </si>
-  <si>
-    <t>06111997</t>
-  </si>
-  <si>
-    <t>Madurai</t>
-  </si>
-  <si>
-    <t>02051995</t>
-  </si>
-  <si>
-    <t>Salem</t>
-  </si>
-  <si>
-    <t>18011997</t>
-  </si>
-  <si>
-    <t>Tiruchirapalli</t>
-  </si>
-  <si>
-    <t>23091998</t>
-  </si>
-  <si>
-    <t>Tirunelveli</t>
-  </si>
-  <si>
-    <t>29011997</t>
-  </si>
-  <si>
-    <t>Vellore</t>
-  </si>
-  <si>
-    <t>16091993</t>
-  </si>
-  <si>
-    <t>Chirala</t>
-  </si>
-  <si>
-    <t>16091992</t>
-  </si>
-  <si>
-    <t>Guntur</t>
-  </si>
-  <si>
-    <t>04091996</t>
+    <t>repotime1</t>
+  </si>
+  <si>
+    <t>gateclose1</t>
+  </si>
+  <si>
+    <t>repotime2</t>
+  </si>
+  <si>
+    <t>gateclose2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shift 1 : 07.45 AM</t>
+  </si>
+  <si>
+    <t>Shift 1 : 08.30 AM</t>
   </si>
 </sst>
 </file>
@@ -639,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD50"/>
+  <dimension ref="A1:BF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,11 +598,13 @@
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="5" width="20" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="39" max="39" width="23.7109375" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" customWidth="1"/>
+    <col min="41" max="41" width="23.7109375" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="1" customFormat="1">
+    <row r="1" spans="1:58" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,860 +629,376 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AP1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AR1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AS1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BB1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BC1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BD1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BE1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BF1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:58" s="1" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:56" s="1" customFormat="1">
-      <c r="A2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="C2" s="1">
-        <v>10001497514</v>
+        <v>10000000003</v>
       </c>
       <c r="D2" s="1">
         <v>8201000001</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="Q2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="R2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="S2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="T2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="U2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="AO2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="BD2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:56" s="1" customFormat="1">
+    </row>
+    <row r="3" spans="1:58" s="1" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1">
-        <v>10003195293</v>
+        <v>10000238381</v>
       </c>
       <c r="D3" s="1">
         <v>8201000002</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="R3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="S3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="U3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="AO3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD3" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56" s="1" customFormat="1">
-      <c r="A4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10003196497</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8201000003</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB4" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD4" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:56" s="1" customFormat="1">
-      <c r="A5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="1">
-        <v>10003295738</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8201000004</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BB5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:56" s="1" customFormat="1">
-      <c r="A6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="1">
-        <v>10003281301</v>
-      </c>
-      <c r="D6" s="1">
-        <v>8201000005</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB6" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD6" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:56" s="1" customFormat="1">
-      <c r="A7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="1">
-        <v>10001094812</v>
-      </c>
-      <c r="D7" s="1">
-        <v>8201000006</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB7" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD7" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:56" s="1" customFormat="1">
-      <c r="A8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="1">
-        <v>71001081535</v>
-      </c>
-      <c r="D8" s="1">
-        <v>8201000007</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BB8" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD8" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:56" s="1" customFormat="1">
-      <c r="A9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10003199296</v>
-      </c>
-      <c r="D9" s="1">
-        <v>8201000008</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BB9" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD9" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:56" s="1" customFormat="1">
-      <c r="A10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10002885552</v>
-      </c>
-      <c r="D10" s="1">
-        <v>8201000009</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BB10" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC10" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD10" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:56" s="1" customFormat="1">
-      <c r="A11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10002784399</v>
-      </c>
-      <c r="D11" s="1">
-        <v>8201000010</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="BB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC11" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD11" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:56" s="1" customFormat="1">
-      <c r="A12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10002692196</v>
-      </c>
-      <c r="D12" s="1">
-        <v>8201000011</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM12" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="BB12" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC12" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD12" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:56" s="1" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="1">
-        <v>71000285455</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8201000012</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM13" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="BB13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD13" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:56">
+    </row>
+    <row r="4" spans="1:58" s="1" customFormat="1">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="G4" s="2"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="AO4" s="4"/>
+      <c r="BF4" s="4"/>
+    </row>
+    <row r="5" spans="1:58" s="1" customFormat="1">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="AO5" s="4"/>
+      <c r="BF5" s="4"/>
+    </row>
+    <row r="6" spans="1:58" s="1" customFormat="1">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="AO6" s="4"/>
+      <c r="BF6" s="4"/>
+    </row>
+    <row r="7" spans="1:58" s="1" customFormat="1">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="AO7" s="4"/>
+      <c r="BF7" s="4"/>
+    </row>
+    <row r="8" spans="1:58" s="1" customFormat="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="AO8" s="4"/>
+      <c r="BF8" s="4"/>
+    </row>
+    <row r="9" spans="1:58" s="1" customFormat="1">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="AO9" s="4"/>
+      <c r="BF9" s="4"/>
+    </row>
+    <row r="10" spans="1:58" s="1" customFormat="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="AO10" s="4"/>
+      <c r="BF10" s="4"/>
+    </row>
+    <row r="11" spans="1:58" s="1" customFormat="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="AO11" s="4"/>
+      <c r="BF11" s="4"/>
+    </row>
+    <row r="12" spans="1:58" s="1" customFormat="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="AO12" s="4"/>
+      <c r="BF12" s="4"/>
+    </row>
+    <row r="13" spans="1:58" s="1" customFormat="1">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="AO13" s="4"/>
+      <c r="BF13" s="4"/>
+    </row>
+    <row r="14" spans="1:58">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="1"/>
@@ -1549,14 +1013,14 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="5"/>
+      <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
+      <c r="V14" s="5"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -1573,9 +1037,9 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
-      <c r="AM14" s="4"/>
+      <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
-      <c r="AO14" s="1"/>
+      <c r="AO14" s="4"/>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
       <c r="AR14" s="1"/>
@@ -1590,9 +1054,11 @@
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
       <c r="BC14" s="1"/>
-      <c r="BD14" s="4"/>
-    </row>
-    <row r="15" spans="1:56">
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="4"/>
+    </row>
+    <row r="15" spans="1:58">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="1"/>
@@ -1607,14 +1073,14 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="5"/>
+      <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
+      <c r="V15" s="5"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
@@ -1631,9 +1097,9 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
-      <c r="AM15" s="4"/>
+      <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
-      <c r="AO15" s="1"/>
+      <c r="AO15" s="4"/>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
       <c r="AR15" s="1"/>
@@ -1648,9 +1114,11 @@
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
       <c r="BC15" s="1"/>
-      <c r="BD15" s="4"/>
-    </row>
-    <row r="16" spans="1:56">
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="4"/>
+    </row>
+    <row r="16" spans="1:58">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="1"/>
@@ -1665,14 +1133,14 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="5"/>
+      <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
+      <c r="V16" s="5"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
@@ -1689,9 +1157,9 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
-      <c r="AM16" s="4"/>
+      <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
-      <c r="AO16" s="1"/>
+      <c r="AO16" s="4"/>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="AR16" s="1"/>
@@ -1706,9 +1174,11 @@
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
       <c r="BC16" s="1"/>
-      <c r="BD16" s="4"/>
-    </row>
-    <row r="17" spans="1:56">
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="4"/>
+    </row>
+    <row r="17" spans="1:58">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="1"/>
@@ -1723,14 +1193,14 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="5"/>
+      <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
+      <c r="V17" s="5"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
@@ -1747,9 +1217,9 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
-      <c r="AM17" s="4"/>
+      <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
-      <c r="AO17" s="1"/>
+      <c r="AO17" s="4"/>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
@@ -1764,9 +1234,11 @@
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
       <c r="BC17" s="1"/>
-      <c r="BD17" s="4"/>
-    </row>
-    <row r="18" spans="1:56">
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="4"/>
+    </row>
+    <row r="18" spans="1:58">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="1"/>
@@ -1781,14 +1253,14 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="5"/>
+      <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
+      <c r="V18" s="5"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -1805,9 +1277,9 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
-      <c r="AM18" s="4"/>
+      <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
-      <c r="AO18" s="1"/>
+      <c r="AO18" s="4"/>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
       <c r="AR18" s="1"/>
@@ -1822,9 +1294,11 @@
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
       <c r="BC18" s="1"/>
-      <c r="BD18" s="4"/>
-    </row>
-    <row r="19" spans="1:56">
+      <c r="BD18" s="1"/>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="4"/>
+    </row>
+    <row r="19" spans="1:58">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="1"/>
@@ -1839,14 +1313,14 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="5"/>
+      <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
+      <c r="V19" s="5"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -1863,9 +1337,9 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
-      <c r="AM19" s="4"/>
+      <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
-      <c r="AO19" s="1"/>
+      <c r="AO19" s="4"/>
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
       <c r="AR19" s="1"/>
@@ -1880,9 +1354,11 @@
       <c r="BA19" s="1"/>
       <c r="BB19" s="1"/>
       <c r="BC19" s="1"/>
-      <c r="BD19" s="4"/>
-    </row>
-    <row r="20" spans="1:56">
+      <c r="BD19" s="1"/>
+      <c r="BE19" s="1"/>
+      <c r="BF19" s="4"/>
+    </row>
+    <row r="20" spans="1:58">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="1"/>
@@ -1897,14 +1373,14 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="5"/>
+      <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
+      <c r="V20" s="5"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -1921,9 +1397,9 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="1"/>
-      <c r="AM20" s="4"/>
+      <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
-      <c r="AO20" s="1"/>
+      <c r="AO20" s="4"/>
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
       <c r="AR20" s="1"/>
@@ -1938,9 +1414,11 @@
       <c r="BA20" s="1"/>
       <c r="BB20" s="1"/>
       <c r="BC20" s="1"/>
-      <c r="BD20" s="4"/>
-    </row>
-    <row r="21" spans="1:56">
+      <c r="BD20" s="1"/>
+      <c r="BE20" s="1"/>
+      <c r="BF20" s="4"/>
+    </row>
+    <row r="21" spans="1:58">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="1"/>
@@ -1955,14 +1433,14 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="5"/>
+      <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
+      <c r="V21" s="5"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
@@ -1979,9 +1457,9 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
-      <c r="AM21" s="4"/>
+      <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
-      <c r="AO21" s="1"/>
+      <c r="AO21" s="4"/>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
       <c r="AR21" s="1"/>
@@ -1996,9 +1474,11 @@
       <c r="BA21" s="1"/>
       <c r="BB21" s="1"/>
       <c r="BC21" s="1"/>
-      <c r="BD21" s="4"/>
-    </row>
-    <row r="22" spans="1:56">
+      <c r="BD21" s="1"/>
+      <c r="BE21" s="1"/>
+      <c r="BF21" s="4"/>
+    </row>
+    <row r="22" spans="1:58">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="1"/>
@@ -2013,14 +1493,14 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="5"/>
+      <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
+      <c r="V22" s="5"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
@@ -2037,9 +1517,9 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
-      <c r="AM22" s="4"/>
+      <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
-      <c r="AO22" s="1"/>
+      <c r="AO22" s="4"/>
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
@@ -2054,9 +1534,11 @@
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
       <c r="BC22" s="1"/>
-      <c r="BD22" s="4"/>
-    </row>
-    <row r="23" spans="1:56">
+      <c r="BD22" s="1"/>
+      <c r="BE22" s="1"/>
+      <c r="BF22" s="4"/>
+    </row>
+    <row r="23" spans="1:58">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="1"/>
@@ -2071,14 +1553,14 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="5"/>
+      <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
+      <c r="V23" s="5"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -2095,9 +1577,9 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
       <c r="AL23" s="1"/>
-      <c r="AM23" s="4"/>
+      <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
-      <c r="AO23" s="1"/>
+      <c r="AO23" s="4"/>
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
       <c r="AR23" s="1"/>
@@ -2112,9 +1594,11 @@
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
       <c r="BC23" s="1"/>
-      <c r="BD23" s="4"/>
-    </row>
-    <row r="24" spans="1:56">
+      <c r="BD23" s="1"/>
+      <c r="BE23" s="1"/>
+      <c r="BF23" s="4"/>
+    </row>
+    <row r="24" spans="1:58">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="1"/>
@@ -2129,14 +1613,14 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="5"/>
+      <c r="T24" s="1"/>
       <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
+      <c r="V24" s="5"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
@@ -2153,9 +1637,9 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
-      <c r="AM24" s="4"/>
+      <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
-      <c r="AO24" s="1"/>
+      <c r="AO24" s="4"/>
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1"/>
@@ -2170,9 +1654,11 @@
       <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
       <c r="BC24" s="1"/>
-      <c r="BD24" s="4"/>
-    </row>
-    <row r="25" spans="1:56">
+      <c r="BD24" s="1"/>
+      <c r="BE24" s="1"/>
+      <c r="BF24" s="4"/>
+    </row>
+    <row r="25" spans="1:58">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="1"/>
@@ -2187,14 +1673,14 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="5"/>
+      <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
+      <c r="V25" s="5"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -2211,9 +1697,9 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
-      <c r="AM25" s="4"/>
+      <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
-      <c r="AO25" s="1"/>
+      <c r="AO25" s="4"/>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
       <c r="AR25" s="1"/>
@@ -2228,9 +1714,11 @@
       <c r="BA25" s="1"/>
       <c r="BB25" s="1"/>
       <c r="BC25" s="1"/>
-      <c r="BD25" s="4"/>
-    </row>
-    <row r="26" spans="1:56">
+      <c r="BD25" s="1"/>
+      <c r="BE25" s="1"/>
+      <c r="BF25" s="4"/>
+    </row>
+    <row r="26" spans="1:58">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="1"/>
@@ -2245,14 +1733,14 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="5"/>
+      <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
+      <c r="V26" s="5"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
@@ -2269,9 +1757,9 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
-      <c r="AM26" s="4"/>
+      <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
-      <c r="AO26" s="1"/>
+      <c r="AO26" s="4"/>
       <c r="AP26" s="1"/>
       <c r="AQ26" s="1"/>
       <c r="AR26" s="1"/>
@@ -2286,9 +1774,11 @@
       <c r="BA26" s="1"/>
       <c r="BB26" s="1"/>
       <c r="BC26" s="1"/>
-      <c r="BD26" s="4"/>
-    </row>
-    <row r="27" spans="1:56">
+      <c r="BD26" s="1"/>
+      <c r="BE26" s="1"/>
+      <c r="BF26" s="4"/>
+    </row>
+    <row r="27" spans="1:58">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="1"/>
@@ -2303,14 +1793,14 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
       <c r="S27" s="1"/>
-      <c r="T27" s="5"/>
+      <c r="T27" s="1"/>
       <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
+      <c r="V27" s="5"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
@@ -2327,9 +1817,9 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
-      <c r="AM27" s="4"/>
+      <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
-      <c r="AO27" s="1"/>
+      <c r="AO27" s="4"/>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
       <c r="AR27" s="1"/>
@@ -2344,9 +1834,11 @@
       <c r="BA27" s="1"/>
       <c r="BB27" s="1"/>
       <c r="BC27" s="1"/>
-      <c r="BD27" s="4"/>
-    </row>
-    <row r="28" spans="1:56">
+      <c r="BD27" s="1"/>
+      <c r="BE27" s="1"/>
+      <c r="BF27" s="4"/>
+    </row>
+    <row r="28" spans="1:58">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="1"/>
@@ -2361,14 +1853,14 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
       <c r="S28" s="1"/>
-      <c r="T28" s="5"/>
+      <c r="T28" s="1"/>
       <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
+      <c r="V28" s="5"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
@@ -2385,9 +1877,9 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
-      <c r="AM28" s="4"/>
+      <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
-      <c r="AO28" s="1"/>
+      <c r="AO28" s="4"/>
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
@@ -2398,13 +1890,15 @@
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
       <c r="AY28" s="1"/>
-      <c r="AZ28" s="3"/>
-      <c r="BA28" s="3"/>
-      <c r="BB28" s="1"/>
-      <c r="BC28" s="1"/>
-      <c r="BD28" s="4"/>
-    </row>
-    <row r="29" spans="1:56">
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="3"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="4"/>
+    </row>
+    <row r="29" spans="1:58">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="1"/>
@@ -2419,14 +1913,14 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="5"/>
+      <c r="T29" s="1"/>
       <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
+      <c r="V29" s="5"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
@@ -2443,9 +1937,9 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
       <c r="AL29" s="1"/>
-      <c r="AM29" s="4"/>
+      <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
-      <c r="AO29" s="1"/>
+      <c r="AO29" s="4"/>
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
       <c r="AR29" s="1"/>
@@ -2460,9 +1954,11 @@
       <c r="BA29" s="1"/>
       <c r="BB29" s="1"/>
       <c r="BC29" s="1"/>
-      <c r="BD29" s="4"/>
-    </row>
-    <row r="30" spans="1:56">
+      <c r="BD29" s="1"/>
+      <c r="BE29" s="1"/>
+      <c r="BF29" s="4"/>
+    </row>
+    <row r="30" spans="1:58">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="1"/>
@@ -2477,14 +1973,14 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="5"/>
+      <c r="T30" s="1"/>
       <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
+      <c r="V30" s="5"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
@@ -2501,9 +1997,9 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
-      <c r="AM30" s="4"/>
+      <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
-      <c r="AO30" s="1"/>
+      <c r="AO30" s="4"/>
       <c r="AP30" s="1"/>
       <c r="AQ30" s="1"/>
       <c r="AR30" s="1"/>
@@ -2518,9 +2014,11 @@
       <c r="BA30" s="1"/>
       <c r="BB30" s="1"/>
       <c r="BC30" s="1"/>
-      <c r="BD30" s="4"/>
-    </row>
-    <row r="31" spans="1:56">
+      <c r="BD30" s="1"/>
+      <c r="BE30" s="1"/>
+      <c r="BF30" s="4"/>
+    </row>
+    <row r="31" spans="1:58">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="1"/>
@@ -2535,14 +2033,14 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
       <c r="S31" s="1"/>
-      <c r="T31" s="5"/>
+      <c r="T31" s="1"/>
       <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
+      <c r="V31" s="5"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
@@ -2559,9 +2057,9 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
       <c r="AL31" s="1"/>
-      <c r="AM31" s="4"/>
+      <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
-      <c r="AO31" s="1"/>
+      <c r="AO31" s="4"/>
       <c r="AP31" s="1"/>
       <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
@@ -2576,9 +2074,11 @@
       <c r="BA31" s="1"/>
       <c r="BB31" s="1"/>
       <c r="BC31" s="1"/>
-      <c r="BD31" s="4"/>
-    </row>
-    <row r="32" spans="1:56">
+      <c r="BD31" s="1"/>
+      <c r="BE31" s="1"/>
+      <c r="BF31" s="4"/>
+    </row>
+    <row r="32" spans="1:58">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="1"/>
@@ -2593,14 +2093,14 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="5"/>
+      <c r="T32" s="1"/>
       <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
+      <c r="V32" s="5"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -2617,9 +2117,9 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
-      <c r="AM32" s="4"/>
+      <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
-      <c r="AO32" s="1"/>
+      <c r="AO32" s="4"/>
       <c r="AP32" s="1"/>
       <c r="AQ32" s="1"/>
       <c r="AR32" s="1"/>
@@ -2634,9 +2134,11 @@
       <c r="BA32" s="1"/>
       <c r="BB32" s="1"/>
       <c r="BC32" s="1"/>
-      <c r="BD32" s="4"/>
-    </row>
-    <row r="33" spans="1:56">
+      <c r="BD32" s="1"/>
+      <c r="BE32" s="1"/>
+      <c r="BF32" s="4"/>
+    </row>
+    <row r="33" spans="1:58">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="1"/>
@@ -2651,14 +2153,14 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
       <c r="S33" s="1"/>
-      <c r="T33" s="5"/>
+      <c r="T33" s="1"/>
       <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
+      <c r="V33" s="5"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
@@ -2675,9 +2177,9 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
-      <c r="AM33" s="4"/>
+      <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
-      <c r="AO33" s="1"/>
+      <c r="AO33" s="4"/>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
       <c r="AR33" s="1"/>
@@ -2692,9 +2194,11 @@
       <c r="BA33" s="1"/>
       <c r="BB33" s="1"/>
       <c r="BC33" s="1"/>
-      <c r="BD33" s="4"/>
-    </row>
-    <row r="34" spans="1:56">
+      <c r="BD33" s="1"/>
+      <c r="BE33" s="1"/>
+      <c r="BF33" s="4"/>
+    </row>
+    <row r="34" spans="1:58">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="1"/>
@@ -2709,14 +2213,14 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
       <c r="S34" s="1"/>
-      <c r="T34" s="5"/>
+      <c r="T34" s="1"/>
       <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
+      <c r="V34" s="5"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
@@ -2733,9 +2237,9 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
-      <c r="AM34" s="4"/>
+      <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
-      <c r="AO34" s="1"/>
+      <c r="AO34" s="4"/>
       <c r="AP34" s="1"/>
       <c r="AQ34" s="1"/>
       <c r="AR34" s="1"/>
@@ -2750,9 +2254,11 @@
       <c r="BA34" s="1"/>
       <c r="BB34" s="1"/>
       <c r="BC34" s="1"/>
-      <c r="BD34" s="4"/>
-    </row>
-    <row r="35" spans="1:56">
+      <c r="BD34" s="1"/>
+      <c r="BE34" s="1"/>
+      <c r="BF34" s="4"/>
+    </row>
+    <row r="35" spans="1:58">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="1"/>
@@ -2767,14 +2273,14 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
       <c r="S35" s="1"/>
-      <c r="T35" s="5"/>
+      <c r="T35" s="1"/>
       <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
+      <c r="V35" s="5"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
@@ -2791,9 +2297,9 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
       <c r="AL35" s="1"/>
-      <c r="AM35" s="4"/>
+      <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
-      <c r="AO35" s="1"/>
+      <c r="AO35" s="4"/>
       <c r="AP35" s="1"/>
       <c r="AQ35" s="1"/>
       <c r="AR35" s="1"/>
@@ -2808,9 +2314,11 @@
       <c r="BA35" s="1"/>
       <c r="BB35" s="1"/>
       <c r="BC35" s="1"/>
-      <c r="BD35" s="4"/>
-    </row>
-    <row r="36" spans="1:56">
+      <c r="BD35" s="1"/>
+      <c r="BE35" s="1"/>
+      <c r="BF35" s="4"/>
+    </row>
+    <row r="36" spans="1:58">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="1"/>
@@ -2825,14 +2333,14 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
       <c r="S36" s="1"/>
-      <c r="T36" s="5"/>
+      <c r="T36" s="1"/>
       <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
+      <c r="V36" s="5"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
@@ -2849,9 +2357,9 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
       <c r="AL36" s="1"/>
-      <c r="AM36" s="4"/>
+      <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
-      <c r="AO36" s="1"/>
+      <c r="AO36" s="4"/>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
       <c r="AR36" s="1"/>
@@ -2866,9 +2374,11 @@
       <c r="BA36" s="1"/>
       <c r="BB36" s="1"/>
       <c r="BC36" s="1"/>
-      <c r="BD36" s="4"/>
-    </row>
-    <row r="37" spans="1:56">
+      <c r="BD36" s="1"/>
+      <c r="BE36" s="1"/>
+      <c r="BF36" s="4"/>
+    </row>
+    <row r="37" spans="1:58">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="1"/>
@@ -2883,14 +2393,14 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
       <c r="S37" s="1"/>
-      <c r="T37" s="5"/>
+      <c r="T37" s="1"/>
       <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
+      <c r="V37" s="5"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
@@ -2907,9 +2417,9 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
       <c r="AL37" s="1"/>
-      <c r="AM37" s="4"/>
+      <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
-      <c r="AO37" s="1"/>
+      <c r="AO37" s="4"/>
       <c r="AP37" s="1"/>
       <c r="AQ37" s="1"/>
       <c r="AR37" s="1"/>
@@ -2924,9 +2434,11 @@
       <c r="BA37" s="1"/>
       <c r="BB37" s="1"/>
       <c r="BC37" s="1"/>
-      <c r="BD37" s="4"/>
-    </row>
-    <row r="38" spans="1:56">
+      <c r="BD37" s="1"/>
+      <c r="BE37" s="1"/>
+      <c r="BF37" s="4"/>
+    </row>
+    <row r="38" spans="1:58">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2941,14 +2453,14 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
       <c r="S38" s="1"/>
-      <c r="T38" s="5"/>
+      <c r="T38" s="1"/>
       <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
+      <c r="V38" s="5"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
@@ -2965,9 +2477,9 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
       <c r="AL38" s="1"/>
-      <c r="AM38" s="4"/>
+      <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
-      <c r="AO38" s="1"/>
+      <c r="AO38" s="4"/>
       <c r="AP38" s="1"/>
       <c r="AQ38" s="1"/>
       <c r="AR38" s="1"/>
@@ -2982,9 +2494,11 @@
       <c r="BA38" s="1"/>
       <c r="BB38" s="1"/>
       <c r="BC38" s="1"/>
-      <c r="BD38" s="4"/>
-    </row>
-    <row r="39" spans="1:56">
+      <c r="BD38" s="1"/>
+      <c r="BE38" s="1"/>
+      <c r="BF38" s="4"/>
+    </row>
+    <row r="39" spans="1:58">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="1"/>
@@ -2999,14 +2513,14 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
       <c r="S39" s="1"/>
-      <c r="T39" s="5"/>
+      <c r="T39" s="1"/>
       <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
+      <c r="V39" s="5"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
@@ -3023,9 +2537,9 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
       <c r="AL39" s="1"/>
-      <c r="AM39" s="4"/>
+      <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
-      <c r="AO39" s="1"/>
+      <c r="AO39" s="4"/>
       <c r="AP39" s="1"/>
       <c r="AQ39" s="1"/>
       <c r="AR39" s="1"/>
@@ -3040,9 +2554,11 @@
       <c r="BA39" s="1"/>
       <c r="BB39" s="1"/>
       <c r="BC39" s="1"/>
-      <c r="BD39" s="4"/>
-    </row>
-    <row r="40" spans="1:56">
+      <c r="BD39" s="1"/>
+      <c r="BE39" s="1"/>
+      <c r="BF39" s="4"/>
+    </row>
+    <row r="40" spans="1:58">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="1"/>
@@ -3057,14 +2573,14 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
       <c r="S40" s="1"/>
-      <c r="T40" s="5"/>
+      <c r="T40" s="1"/>
       <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
+      <c r="V40" s="5"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
@@ -3081,9 +2597,9 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
       <c r="AL40" s="1"/>
-      <c r="AM40" s="4"/>
+      <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
-      <c r="AO40" s="1"/>
+      <c r="AO40" s="4"/>
       <c r="AP40" s="1"/>
       <c r="AQ40" s="1"/>
       <c r="AR40" s="1"/>
@@ -3098,9 +2614,11 @@
       <c r="BA40" s="1"/>
       <c r="BB40" s="1"/>
       <c r="BC40" s="1"/>
-      <c r="BD40" s="4"/>
-    </row>
-    <row r="41" spans="1:56">
+      <c r="BD40" s="1"/>
+      <c r="BE40" s="1"/>
+      <c r="BF40" s="4"/>
+    </row>
+    <row r="41" spans="1:58">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="1"/>
@@ -3115,14 +2633,14 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
       <c r="S41" s="1"/>
-      <c r="T41" s="5"/>
+      <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
+      <c r="V41" s="5"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
@@ -3139,9 +2657,9 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
       <c r="AL41" s="1"/>
-      <c r="AM41" s="4"/>
+      <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
-      <c r="AO41" s="1"/>
+      <c r="AO41" s="4"/>
       <c r="AP41" s="1"/>
       <c r="AQ41" s="1"/>
       <c r="AR41" s="1"/>
@@ -3156,9 +2674,11 @@
       <c r="BA41" s="1"/>
       <c r="BB41" s="1"/>
       <c r="BC41" s="1"/>
-      <c r="BD41" s="4"/>
-    </row>
-    <row r="42" spans="1:56">
+      <c r="BD41" s="1"/>
+      <c r="BE41" s="1"/>
+      <c r="BF41" s="4"/>
+    </row>
+    <row r="42" spans="1:58">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="1"/>
@@ -3173,14 +2693,14 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
       <c r="S42" s="1"/>
-      <c r="T42" s="5"/>
+      <c r="T42" s="1"/>
       <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
+      <c r="V42" s="5"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
@@ -3197,9 +2717,9 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
       <c r="AL42" s="1"/>
-      <c r="AM42" s="4"/>
+      <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
-      <c r="AO42" s="1"/>
+      <c r="AO42" s="4"/>
       <c r="AP42" s="1"/>
       <c r="AQ42" s="1"/>
       <c r="AR42" s="1"/>
@@ -3214,9 +2734,11 @@
       <c r="BA42" s="1"/>
       <c r="BB42" s="1"/>
       <c r="BC42" s="1"/>
-      <c r="BD42" s="4"/>
-    </row>
-    <row r="43" spans="1:56">
+      <c r="BD42" s="1"/>
+      <c r="BE42" s="1"/>
+      <c r="BF42" s="4"/>
+    </row>
+    <row r="43" spans="1:58">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="1"/>
@@ -3231,14 +2753,14 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
       <c r="S43" s="1"/>
-      <c r="T43" s="5"/>
+      <c r="T43" s="1"/>
       <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
+      <c r="V43" s="5"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -3255,9 +2777,9 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
       <c r="AL43" s="1"/>
-      <c r="AM43" s="4"/>
+      <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
-      <c r="AO43" s="1"/>
+      <c r="AO43" s="4"/>
       <c r="AP43" s="1"/>
       <c r="AQ43" s="1"/>
       <c r="AR43" s="1"/>
@@ -3272,9 +2794,11 @@
       <c r="BA43" s="1"/>
       <c r="BB43" s="1"/>
       <c r="BC43" s="1"/>
-      <c r="BD43" s="4"/>
-    </row>
-    <row r="44" spans="1:56">
+      <c r="BD43" s="1"/>
+      <c r="BE43" s="1"/>
+      <c r="BF43" s="4"/>
+    </row>
+    <row r="44" spans="1:58">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="1"/>
@@ -3289,14 +2813,14 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="5"/>
+      <c r="T44" s="1"/>
       <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
+      <c r="V44" s="5"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -3313,9 +2837,9 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
       <c r="AL44" s="1"/>
-      <c r="AM44" s="4"/>
+      <c r="AM44" s="1"/>
       <c r="AN44" s="1"/>
-      <c r="AO44" s="1"/>
+      <c r="AO44" s="4"/>
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
       <c r="AR44" s="1"/>
@@ -3330,9 +2854,11 @@
       <c r="BA44" s="1"/>
       <c r="BB44" s="1"/>
       <c r="BC44" s="1"/>
-      <c r="BD44" s="4"/>
-    </row>
-    <row r="45" spans="1:56">
+      <c r="BD44" s="1"/>
+      <c r="BE44" s="1"/>
+      <c r="BF44" s="4"/>
+    </row>
+    <row r="45" spans="1:58">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="1"/>
@@ -3347,14 +2873,14 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
       <c r="S45" s="1"/>
-      <c r="T45" s="5"/>
+      <c r="T45" s="1"/>
       <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
+      <c r="V45" s="5"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
@@ -3371,9 +2897,9 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
       <c r="AL45" s="1"/>
-      <c r="AM45" s="4"/>
+      <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
-      <c r="AO45" s="1"/>
+      <c r="AO45" s="4"/>
       <c r="AP45" s="1"/>
       <c r="AQ45" s="1"/>
       <c r="AR45" s="1"/>
@@ -3388,9 +2914,11 @@
       <c r="BA45" s="1"/>
       <c r="BB45" s="1"/>
       <c r="BC45" s="1"/>
-      <c r="BD45" s="4"/>
-    </row>
-    <row r="46" spans="1:56">
+      <c r="BD45" s="1"/>
+      <c r="BE45" s="1"/>
+      <c r="BF45" s="4"/>
+    </row>
+    <row r="46" spans="1:58">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="1"/>
@@ -3405,14 +2933,14 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
       <c r="S46" s="1"/>
-      <c r="T46" s="5"/>
+      <c r="T46" s="1"/>
       <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
+      <c r="V46" s="5"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
@@ -3429,9 +2957,9 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
       <c r="AL46" s="1"/>
-      <c r="AM46" s="4"/>
+      <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
-      <c r="AO46" s="1"/>
+      <c r="AO46" s="4"/>
       <c r="AP46" s="1"/>
       <c r="AQ46" s="1"/>
       <c r="AR46" s="1"/>
@@ -3446,9 +2974,11 @@
       <c r="BA46" s="1"/>
       <c r="BB46" s="1"/>
       <c r="BC46" s="1"/>
-      <c r="BD46" s="4"/>
-    </row>
-    <row r="47" spans="1:56">
+      <c r="BD46" s="1"/>
+      <c r="BE46" s="1"/>
+      <c r="BF46" s="4"/>
+    </row>
+    <row r="47" spans="1:58">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="1"/>
@@ -3463,14 +2993,14 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
       <c r="S47" s="1"/>
-      <c r="T47" s="5"/>
+      <c r="T47" s="1"/>
       <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
+      <c r="V47" s="5"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
@@ -3487,9 +3017,9 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
       <c r="AL47" s="1"/>
-      <c r="AM47" s="4"/>
+      <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
-      <c r="AO47" s="1"/>
+      <c r="AO47" s="4"/>
       <c r="AP47" s="1"/>
       <c r="AQ47" s="1"/>
       <c r="AR47" s="1"/>
@@ -3504,9 +3034,11 @@
       <c r="BA47" s="1"/>
       <c r="BB47" s="1"/>
       <c r="BC47" s="1"/>
-      <c r="BD47" s="4"/>
-    </row>
-    <row r="48" spans="1:56">
+      <c r="BD47" s="1"/>
+      <c r="BE47" s="1"/>
+      <c r="BF47" s="4"/>
+    </row>
+    <row r="48" spans="1:58">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="1"/>
@@ -3521,14 +3053,14 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
       <c r="S48" s="1"/>
-      <c r="T48" s="5"/>
+      <c r="T48" s="1"/>
       <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
+      <c r="V48" s="5"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
@@ -3545,9 +3077,9 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
       <c r="AL48" s="1"/>
-      <c r="AM48" s="4"/>
+      <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
-      <c r="AO48" s="1"/>
+      <c r="AO48" s="4"/>
       <c r="AP48" s="1"/>
       <c r="AQ48" s="1"/>
       <c r="AR48" s="1"/>
@@ -3562,9 +3094,11 @@
       <c r="BA48" s="1"/>
       <c r="BB48" s="1"/>
       <c r="BC48" s="1"/>
-      <c r="BD48" s="4"/>
-    </row>
-    <row r="49" spans="1:56">
+      <c r="BD48" s="1"/>
+      <c r="BE48" s="1"/>
+      <c r="BF48" s="4"/>
+    </row>
+    <row r="49" spans="1:58">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="1"/>
@@ -3579,14 +3113,14 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
       <c r="S49" s="1"/>
-      <c r="T49" s="5"/>
+      <c r="T49" s="1"/>
       <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
+      <c r="V49" s="5"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
@@ -3603,9 +3137,9 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
       <c r="AL49" s="1"/>
-      <c r="AM49" s="4"/>
+      <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
-      <c r="AO49" s="1"/>
+      <c r="AO49" s="4"/>
       <c r="AP49" s="1"/>
       <c r="AQ49" s="1"/>
       <c r="AR49" s="1"/>
@@ -3620,9 +3154,11 @@
       <c r="BA49" s="1"/>
       <c r="BB49" s="1"/>
       <c r="BC49" s="1"/>
-      <c r="BD49" s="4"/>
-    </row>
-    <row r="50" spans="1:56">
+      <c r="BD49" s="1"/>
+      <c r="BE49" s="1"/>
+      <c r="BF49" s="4"/>
+    </row>
+    <row r="50" spans="1:58">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="1"/>
@@ -3637,14 +3173,14 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
       <c r="S50" s="1"/>
-      <c r="T50" s="5"/>
+      <c r="T50" s="1"/>
       <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
+      <c r="V50" s="5"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
@@ -3661,9 +3197,9 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
       <c r="AL50" s="1"/>
-      <c r="AM50" s="4"/>
+      <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
-      <c r="AO50" s="1"/>
+      <c r="AO50" s="4"/>
       <c r="AP50" s="1"/>
       <c r="AQ50" s="1"/>
       <c r="AR50" s="1"/>
@@ -3678,7 +3214,9 @@
       <c r="BA50" s="1"/>
       <c r="BB50" s="1"/>
       <c r="BC50" s="1"/>
-      <c r="BD50" s="4"/>
+      <c r="BD50" s="1"/>
+      <c r="BE50" s="1"/>
+      <c r="BF50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>